<commit_message>
Finished data cleaning, and added dashborad. Next task is to add readme.
</commit_message>
<xml_diff>
--- a/Tree_data_tables.xlsx
+++ b/Tree_data_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmedina\Documents\Projects\Colle_Park_Residential_Tree_Planting_PRogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F67F3D89-F6C0-47C1-8B21-2B4F72B035A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534F1CE3-3F22-4D88-94F9-49088FBE6C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01886EB5-8083-405C-9AEB-B8EEC5993FA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{01886EB5-8083-405C-9AEB-B8EEC5993FA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Growth_type" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Annual_sequestration_hardwood" sheetId="4" r:id="rId3"/>
     <sheet name="Annual_sequestration_conifer" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Growth_type!$A$1:$D$101</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -382,96 +385,21 @@
     <t>C</t>
   </si>
   <si>
-    <t>Common Name</t>
-  </si>
-  <si>
     <t>Ailanthus</t>
   </si>
   <si>
-    <t xml:space="preserve"> European Alder</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Green Ash</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American  Mountain Ash</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> White Ash</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bigtooth Aspen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quaking Aspen</t>
-  </si>
-  <si>
     <t>Baldcypress</t>
   </si>
   <si>
-    <t xml:space="preserve"> American Beech</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paper (White) Birch</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> River Birch</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yellow Birch</t>
-  </si>
-  <si>
     <t>Boxelder</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ohio Buckeye</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Northern Catalpa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Black Cherry</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pin Cherry</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eastern Cottonwood</t>
-  </si>
-  <si>
     <t>Crabapple</t>
   </si>
   <si>
     <t>Cucumbertree</t>
   </si>
   <si>
-    <t xml:space="preserve"> Flowering Dogwood</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American Elm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chinese Elm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rock Elm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> September Elm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Siberian Elm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Slippery Elm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Balsam Fir</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Douglas Fir</t>
-  </si>
-  <si>
     <t>Ginkgo</t>
   </si>
   <si>
@@ -481,180 +409,18 @@
     <t>Hawthorne</t>
   </si>
   <si>
-    <t xml:space="preserve"> Eastern Hemlock</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bitternut Hickory</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mockernut Hickory</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shagbark Hickory</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shellbark Hickory</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pignut Hickory</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American Holly</t>
-  </si>
-  <si>
     <t>Honeylocust</t>
   </si>
   <si>
-    <t xml:space="preserve"> Eastern Hophornbeam</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Common Horsechestnut</t>
-  </si>
-  <si>
     <t>Kentucky coffeetree</t>
   </si>
   <si>
-    <t xml:space="preserve"> Little-Leaf Linden</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Black Locust</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Southern Magnolia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bigleaf  Maple</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Norway Maple</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Red Maple</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Silver Maple</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sugar Maple</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Red  Mulberry</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Black Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Blue Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bur Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> California Black  Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> California White Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Canyon Live Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chestnut Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chinkapin Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Laurel Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Live Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Northern Red Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Overcup  Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pin Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Scarlet Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Swamp White Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Water Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> White Oak</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Willow Oak</t>
-  </si>
-  <si>
     <t>Pecan</t>
   </si>
   <si>
-    <t xml:space="preserve"> European Black Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jack Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Loblolly Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Longleaf Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ponderosa  Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Red Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Scotch Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shortleaf Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Slash Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Virginia Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> White Eastern Pine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yellow Poplar</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eastern Redbud</t>
-  </si>
-  <si>
     <t>Sassafras</t>
   </si>
   <si>
-    <t xml:space="preserve"> Black Spruce</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Blue  Spruce</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Norway Spruce</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Red Spruce</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> White Spruce</t>
-  </si>
-  <si>
     <t>Sugarberry</t>
   </si>
   <si>
@@ -667,12 +433,6 @@
     <t>Tamarack</t>
   </si>
   <si>
-    <t xml:space="preserve"> Black Walnut</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Black Willow</t>
-  </si>
-  <si>
     <t>Years</t>
   </si>
   <si>
@@ -688,13 +448,256 @@
     <t>Basswood, American, Tilia americana</t>
   </si>
   <si>
-    <t xml:space="preserve"> American Basswood</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eastern Red Cedar</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Northern White Cedar</t>
+    <t>European Alder</t>
+  </si>
+  <si>
+    <t>Green Ash</t>
+  </si>
+  <si>
+    <t>American Mountain Ash</t>
+  </si>
+  <si>
+    <t>White Ash</t>
+  </si>
+  <si>
+    <t>Bigtooth Aspen</t>
+  </si>
+  <si>
+    <t>Quaking Aspen</t>
+  </si>
+  <si>
+    <t>American Basswood</t>
+  </si>
+  <si>
+    <t>American Beech</t>
+  </si>
+  <si>
+    <t>Paper (White) Birch</t>
+  </si>
+  <si>
+    <t>River Birch</t>
+  </si>
+  <si>
+    <t>Yellow Birch</t>
+  </si>
+  <si>
+    <t>Ohio Buckeye</t>
+  </si>
+  <si>
+    <t>Northern Catalpa</t>
+  </si>
+  <si>
+    <t>Eastern Red Cedar</t>
+  </si>
+  <si>
+    <t>Northern White Cedar</t>
+  </si>
+  <si>
+    <t>Black Cherry</t>
+  </si>
+  <si>
+    <t>Pin Cherry</t>
+  </si>
+  <si>
+    <t>Eastern Cottonwood</t>
+  </si>
+  <si>
+    <t>Flowering Dogwood</t>
+  </si>
+  <si>
+    <t>American Elm</t>
+  </si>
+  <si>
+    <t>Chinese Elm</t>
+  </si>
+  <si>
+    <t>Rock Elm</t>
+  </si>
+  <si>
+    <t>September Elm</t>
+  </si>
+  <si>
+    <t>Siberian Elm</t>
+  </si>
+  <si>
+    <t>Slippery Elm</t>
+  </si>
+  <si>
+    <t>Balsam Fir</t>
+  </si>
+  <si>
+    <t>Douglas Fir</t>
+  </si>
+  <si>
+    <t>Eastern Hemlock</t>
+  </si>
+  <si>
+    <t>Bitternut Hickory</t>
+  </si>
+  <si>
+    <t>Mockernut Hickory</t>
+  </si>
+  <si>
+    <t>Shagbark Hickory</t>
+  </si>
+  <si>
+    <t>Shellbark Hickory</t>
+  </si>
+  <si>
+    <t>Pignut Hickory</t>
+  </si>
+  <si>
+    <t>American Holly</t>
+  </si>
+  <si>
+    <t>Eastern Hophornbeam</t>
+  </si>
+  <si>
+    <t>Common Horsechestnut</t>
+  </si>
+  <si>
+    <t>Little-Leaf Linden</t>
+  </si>
+  <si>
+    <t>Black Locust</t>
+  </si>
+  <si>
+    <t>Southern Magnolia</t>
+  </si>
+  <si>
+    <t>Bigleaf Maple</t>
+  </si>
+  <si>
+    <t>Norway Maple</t>
+  </si>
+  <si>
+    <t>Red Maple</t>
+  </si>
+  <si>
+    <t>Silver Maple</t>
+  </si>
+  <si>
+    <t>Sugar Maple</t>
+  </si>
+  <si>
+    <t>Red Mulberry</t>
+  </si>
+  <si>
+    <t>Black Oak</t>
+  </si>
+  <si>
+    <t>Blue Oak</t>
+  </si>
+  <si>
+    <t>Bur Oak</t>
+  </si>
+  <si>
+    <t>California Black Oak</t>
+  </si>
+  <si>
+    <t>California White Oak</t>
+  </si>
+  <si>
+    <t>Canyon Live Oak</t>
+  </si>
+  <si>
+    <t>Chestnut Oak</t>
+  </si>
+  <si>
+    <t>Chinkapin Oak</t>
+  </si>
+  <si>
+    <t>Laurel Oak</t>
+  </si>
+  <si>
+    <t>Live Oak</t>
+  </si>
+  <si>
+    <t>Northern Red Oak</t>
+  </si>
+  <si>
+    <t>Overcup Oak</t>
+  </si>
+  <si>
+    <t>Pin Oak</t>
+  </si>
+  <si>
+    <t>Scarlet Oak</t>
+  </si>
+  <si>
+    <t>Swamp White Oak</t>
+  </si>
+  <si>
+    <t>Water Oak</t>
+  </si>
+  <si>
+    <t>White Oak</t>
+  </si>
+  <si>
+    <t>Willow Oak</t>
+  </si>
+  <si>
+    <t>European Black Pine</t>
+  </si>
+  <si>
+    <t>Jack Pine</t>
+  </si>
+  <si>
+    <t>Loblolly Pine</t>
+  </si>
+  <si>
+    <t>Longleaf Pine</t>
+  </si>
+  <si>
+    <t>Ponderosa Pine</t>
+  </si>
+  <si>
+    <t>Red Pine</t>
+  </si>
+  <si>
+    <t>Scotch Pine</t>
+  </si>
+  <si>
+    <t>Shortleaf Pine</t>
+  </si>
+  <si>
+    <t>Slash Pine</t>
+  </si>
+  <si>
+    <t>Virginia Pine</t>
+  </si>
+  <si>
+    <t>White Eastern Pine</t>
+  </si>
+  <si>
+    <t>Yellow Poplar</t>
+  </si>
+  <si>
+    <t>Eastern Redbud</t>
+  </si>
+  <si>
+    <t>Black Spruce</t>
+  </si>
+  <si>
+    <t>Blue Spruce</t>
+  </si>
+  <si>
+    <t>Norway Spruce</t>
+  </si>
+  <si>
+    <t>Red Spruce</t>
+  </si>
+  <si>
+    <t>White Spruce</t>
+  </si>
+  <si>
+    <t>Black Walnut</t>
+  </si>
+  <si>
+    <t>Black Willow</t>
+  </si>
+  <si>
+    <t>Common name</t>
   </si>
 </sst>
 </file>
@@ -730,9 +733,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,11 +1071,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC6F21C-0E8C-445B-B992-165637732937}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
@@ -1081,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>211</v>
       </c>
       <c r="B1" t="s">
         <v>99</v>
@@ -1095,7 +1099,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -1109,7 +1113,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1123,7 +1127,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1137,7 +1141,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1151,7 +1155,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1165,7 +1169,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -1179,7 +1183,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -1193,7 +1197,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
@@ -1207,10 +1211,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>102</v>
@@ -1221,7 +1225,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -1235,7 +1239,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -1249,7 +1253,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
@@ -1263,7 +1267,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -1277,7 +1281,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1291,7 +1295,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -1305,7 +1309,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
@@ -1319,7 +1323,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
@@ -1333,7 +1337,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>211</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
@@ -1347,7 +1351,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
         <v>45</v>
@@ -1361,7 +1365,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
@@ -1375,7 +1379,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
         <v>49</v>
@@ -1389,7 +1393,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
         <v>51</v>
@@ -1403,7 +1407,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
         <v>53</v>
@@ -1417,7 +1421,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
         <v>55</v>
@@ -1431,7 +1435,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B26" t="s">
         <v>57</v>
@@ -1445,7 +1449,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
@@ -1459,7 +1463,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
         <v>61</v>
@@ -1473,7 +1477,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
         <v>63</v>
@@ -1487,7 +1491,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
@@ -1501,7 +1505,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="B31" t="s">
         <v>67</v>
@@ -1515,7 +1519,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B32" t="s">
         <v>69</v>
@@ -1529,7 +1533,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -1543,7 +1547,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -1557,7 +1561,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -1571,7 +1575,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
@@ -1585,7 +1589,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="B37" t="s">
         <v>71</v>
@@ -1599,7 +1603,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="B38" t="s">
         <v>73</v>
@@ -1613,7 +1617,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="B39" t="s">
         <v>75</v>
@@ -1627,7 +1631,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="B40" t="s">
         <v>77</v>
@@ -1641,7 +1645,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -1655,7 +1659,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B42" t="s">
         <v>79</v>
@@ -1669,7 +1673,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="B43" t="s">
         <v>81</v>
@@ -1683,7 +1687,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="B44" t="s">
         <v>83</v>
@@ -1697,7 +1701,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="B45" t="s">
         <v>85</v>
@@ -1711,7 +1715,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
         <v>87</v>
@@ -1725,7 +1729,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="B47" t="s">
         <v>89</v>
@@ -1739,7 +1743,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B48" t="s">
         <v>91</v>
@@ -1753,7 +1757,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="B49" t="s">
         <v>93</v>
@@ -1781,7 +1785,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
         <v>97</v>
@@ -1795,7 +1799,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="B52" t="s">
         <v>18</v>
@@ -1809,7 +1813,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="B53" t="s">
         <v>4</v>
@@ -1823,7 +1827,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
@@ -1837,7 +1841,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
@@ -1851,7 +1855,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
@@ -1865,7 +1869,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B57" t="s">
         <v>21</v>
@@ -1879,7 +1883,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B58" t="s">
         <v>23</v>
@@ -1893,7 +1897,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="B59" t="s">
         <v>25</v>
@@ -1907,7 +1911,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B60" t="s">
         <v>26</v>
@@ -1921,7 +1925,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
         <v>28</v>
@@ -1935,7 +1939,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
         <v>30</v>
@@ -1949,7 +1953,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
         <v>32</v>
@@ -1963,7 +1967,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="B64" t="s">
         <v>34</v>
@@ -1977,7 +1981,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="B65" t="s">
         <v>36</v>
@@ -1991,7 +1995,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B66" t="s">
         <v>38</v>
@@ -2005,7 +2009,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="B67" t="s">
         <v>40</v>
@@ -2019,7 +2023,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B68" t="s">
         <v>42</v>
@@ -2033,7 +2037,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="B69" t="s">
         <v>44</v>
@@ -2047,7 +2051,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B70" t="s">
         <v>46</v>
@@ -2061,7 +2065,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="B71" t="s">
         <v>48</v>
@@ -2075,7 +2079,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="B72" t="s">
         <v>50</v>
@@ -2089,7 +2093,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
@@ -2103,7 +2107,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="B74" t="s">
         <v>54</v>
@@ -2117,7 +2121,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="B75" t="s">
         <v>56</v>
@@ -2131,7 +2135,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>178</v>
+        <v>117</v>
       </c>
       <c r="B76" t="s">
         <v>58</v>
@@ -2145,7 +2149,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="B77" t="s">
         <v>60</v>
@@ -2159,7 +2163,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="B78" t="s">
         <v>62</v>
@@ -2173,7 +2177,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="B79" t="s">
         <v>64</v>
@@ -2187,7 +2191,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="B80" t="s">
         <v>66</v>
@@ -2201,7 +2205,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B81" t="s">
         <v>68</v>
@@ -2215,7 +2219,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="B82" t="s">
         <v>70</v>
@@ -2229,7 +2233,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
@@ -2243,7 +2247,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="B84" t="s">
         <v>13</v>
@@ -2257,7 +2261,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="B85" t="s">
         <v>14</v>
@@ -2271,7 +2275,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B86" t="s">
         <v>15</v>
@@ -2285,7 +2289,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="B87" t="s">
         <v>72</v>
@@ -2299,7 +2303,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="B88" t="s">
         <v>74</v>
@@ -2313,7 +2317,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="B89" t="s">
         <v>76</v>
@@ -2327,7 +2331,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>192</v>
+        <v>118</v>
       </c>
       <c r="B90" t="s">
         <v>78</v>
@@ -2341,7 +2345,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B91" t="s">
         <v>19</v>
@@ -2355,7 +2359,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B92" t="s">
         <v>80</v>
@@ -2369,7 +2373,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B93" t="s">
         <v>82</v>
@@ -2383,7 +2387,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B94" t="s">
         <v>84</v>
@@ -2397,7 +2401,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="B95" t="s">
         <v>86</v>
@@ -2411,7 +2415,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="B96" t="s">
         <v>88</v>
@@ -2425,7 +2429,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="B97" t="s">
         <v>90</v>
@@ -2439,7 +2443,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>200</v>
+        <v>121</v>
       </c>
       <c r="B98" t="s">
         <v>92</v>
@@ -2453,7 +2457,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>201</v>
+        <v>122</v>
       </c>
       <c r="B99" t="s">
         <v>94</v>
@@ -2467,7 +2471,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="B100" t="s">
         <v>96</v>
@@ -2481,7 +2485,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B101" t="s">
         <v>98</v>
@@ -2494,6 +2498,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D101" xr:uid="{ADC6F21C-0E8C-445B-B992-165637732937}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2502,525 +2507,527 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36E3E11-3252-42D5-81C0-4E01A8B6C6E8}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>205</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>0.873</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.873</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>0.873</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>0.79800000000000004</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.79800000000000004</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>0.79800000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>0.73599999999999999</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0.73599999999999999</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>0.73599999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>0.70599999999999996</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0.70599999999999996</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>0.70599999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>0.67800000000000005</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>0.67800000000000005</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>0.67800000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>0.65800000000000003</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.65800000000000003</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>0.65800000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>0.63900000000000001</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.63900000000000001</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>0.64400000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>0.621</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.621</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>0.63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>0.60299999999999998</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>0.60299999999999998</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>0.61599999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>0.58499999999999996</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>0.58899999999999997</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>0.60199999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>0.56799999999999995</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.57599999999999996</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>0.58899999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>0.55200000000000005</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.56399999999999995</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>0.57599999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>0.53600000000000003</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.55100000000000005</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>0.56299999999999994</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>0.52400000000000002</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.53900000000000003</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>0.55100000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>0.51200000000000001</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>0.52700000000000002</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>0.53900000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>0.501</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.51600000000000001</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>0.52700000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>0.49</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.504</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>0.51600000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>0.47899999999999998</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0.49299999999999999</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>0.505</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>0.46899999999999997</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0.48299999999999998</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>0.495</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>0.45900000000000002</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>0.47199999999999998</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>0.48399999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>0.44800000000000001</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>0.46200000000000002</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>0.47399999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>0.439</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>0.45200000000000001</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>0.46400000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>0.42899999999999999</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>0.442</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>0.45400000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>0.41899999999999998</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>0.433</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>0.44500000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>0.41</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>0.42399999999999999</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>0.435</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>0.40100000000000002</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>0.41499999999999998</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>0.42599999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>0.39200000000000002</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>0.40600000000000003</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>0.41699999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>0.38400000000000001</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>0.39800000000000002</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>0.40899999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>0.375</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>0.38900000000000001</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>0.36699999999999999</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>0.38100000000000001</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>0.39200000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>0.35899999999999999</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>0.373</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>0.38300000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>0.35199999999999998</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>0.36499999999999999</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>0.375</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>0.34399999999999997</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>0.35799999999999998</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>0.36699999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>0.33700000000000002</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>0.35</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>0.36</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36">
         <v>0.33</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
         <v>0.34300000000000003</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36">
         <v>0.34899999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>0.32300000000000001</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>0.33600000000000002</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>0.33900000000000002</v>
       </c>
     </row>
@@ -3033,525 +3040,527 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6D8B99-6761-42F5-9066-45928129CDC2}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>205</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1.3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>1.9</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>2.7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>1.6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>2.7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>3.5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>5.4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>2.4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>4.3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>6.9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>2.8</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>5.2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>8.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>3.2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>6.1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>10.1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>3.7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>7.1</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>11.8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>8.1</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>13.6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>9.1</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>15.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>10.199999999999999</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>17.399999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>5.5</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>11.2</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>19.3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>6</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>12.3</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>21.3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>6.5</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>13.5</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>23.3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>7</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>14.6</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>25.4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>7.5</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>15.8</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>27.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>8.1</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>16.899999999999999</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>29.7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>8.6</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>18.100000000000001</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>31.9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>9.1</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>19.399999999999999</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>34.1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>9.6999999999999993</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>20.6</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>36.299999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>10.199999999999999</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>21.9</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>38.6</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>10.8</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>23.2</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>11.4</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>24.4</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>43.3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>12</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>25.8</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>45.7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>12.5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>27.1</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>48.1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>13.1</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>28.4</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>50.6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>13.7</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>29.8</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>53.1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>14.3</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>31.2</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>55.6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>15</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>32.5</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>58.1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>15.6</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>33.9</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>60.7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>16.2</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>35.299999999999997</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>63.3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>16.8</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>36.799999999999997</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>65.900000000000006</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>17.5</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>38.200000000000003</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>68.5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>18.100000000000001</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>39.700000000000003</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>71.2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>18.7</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>41.1</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>73.8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36">
         <v>19.399999999999999</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
         <v>42.6</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36">
         <v>76.5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>20</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>44.1</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>79.3</v>
       </c>
     </row>
@@ -3564,525 +3573,525 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE04A24F-F0CA-40CE-B110-2CE818F97E19}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>205</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>0.7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>1.4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>0.9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>1.5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>3.1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>1.4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>2.5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>1.6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>3.1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>5.2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>1.9</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>3.7</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>6.4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>7.6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>2.5</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>8.9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>2.8</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>5.8</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>10.199999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>3.1</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>6.6</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>11.7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>3.5</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>7.4</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>13.2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>3.8</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>14.7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>4.2</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>9.1</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>16.3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>9.9</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>17.899999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>10.8</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>19.600000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>5.3</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>11.8</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>21.4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>5.7</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>12.7</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>23.2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>6.1</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>13.7</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>6.6</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>14.7</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>26.9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>7</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>15.7</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>28.8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>7.4</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>16.7</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>30.8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>7.9</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>17.8</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>32.799999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>18.899999999999999</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>34.9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>8.8000000000000007</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>20</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>21.1</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>39.1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>9.6999999999999993</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>22.2</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>41.3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>10.199999999999999</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>23.4</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>43.5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>10.7</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>24.6</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>45.7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>11.2</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>25.8</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>11.7</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>27</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>50.3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>12.2</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>28.2</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>52.7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>12.7</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>29.5</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>55.1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>13.3</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>30.7</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>57.5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>13.8</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>32</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>59.9</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36">
         <v>14.3</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
         <v>33.299999999999997</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36">
         <v>62.4</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>14.9</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>34.700000000000003</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>64.900000000000006</v>
       </c>
     </row>

</xml_diff>